<commit_message>
#40 First date confirmed cases: Guatemala, Cuba, Haiti added & 7 dependencies
Former-commit-id: 880b780a9bfd4deb491bde5ae55d576f1d6c780b
Former-commit-id: 1e2345d19eacb3bac90122705e2cd29be3b3a045
</commit_message>
<xml_diff>
--- a/first date confirmed cases per country.xlsx
+++ b/first date confirmed cases per country.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="19140" windowHeight="7620"/>
+    <workbookView xWindow="1875" yWindow="0" windowWidth="19140" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AA$31</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,55 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t> 1   </t>
-  </si>
-  <si>
-    <t> 2   </t>
-  </si>
-  <si>
-    <t> 4   </t>
-  </si>
-  <si>
-    <t> 5   </t>
-  </si>
-  <si>
-    <t> 6   </t>
-  </si>
-  <si>
-    <t> 7   </t>
-  </si>
-  <si>
-    <t> 8   </t>
-  </si>
-  <si>
-    <t> 9   </t>
-  </si>
-  <si>
-    <t> 10  </t>
-  </si>
-  <si>
-    <t> 11  </t>
-  </si>
-  <si>
-    <t> 12  </t>
-  </si>
-  <si>
-    <t> 13  </t>
-  </si>
-  <si>
-    <t> 14  </t>
-  </si>
-  <si>
-    <t> 15  </t>
-  </si>
-  <si>
-    <t> 16  </t>
-  </si>
-  <si>
-    <t> 17  </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>#</t>
   </si>
@@ -129,6 +84,39 @@
   </si>
   <si>
     <t>FECHA</t>
+  </si>
+  <si>
+    <t>GUATEMALA</t>
+  </si>
+  <si>
+    <t>HAITI</t>
+  </si>
+  <si>
+    <t>CUBA</t>
+  </si>
+  <si>
+    <t>FRENCH GUIANA</t>
+  </si>
+  <si>
+    <t>GUADELOUPE</t>
+  </si>
+  <si>
+    <t>MARTINIQUE</t>
+  </si>
+  <si>
+    <t>PUERTO RICO</t>
+  </si>
+  <si>
+    <t>SAINT MARTIN</t>
+  </si>
+  <si>
+    <t>SAINT BARTHELEMY</t>
+  </si>
+  <si>
+    <t>SAIN PIERRE AND MIQUELON</t>
+  </si>
+  <si>
+    <t>BRAZIL</t>
   </si>
 </sst>
 </file>
@@ -144,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +226,60 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAE4EE4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -291,20 +333,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFAE4EE4"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -579,30 +634,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+      <selection activeCell="B5" sqref="B5:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" customWidth="1"/>
-    <col min="5" max="22" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="3.28515625" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" customWidth="1"/>
+    <col min="9" max="27" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>17</v>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
@@ -623,10 +678,15 @@
       <c r="T1" s="20"/>
       <c r="U1" s="20"/>
       <c r="V1" s="20"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="20">
         <v>2020</v>
       </c>
@@ -649,21 +709,26 @@
       <c r="T2" s="20"/>
       <c r="U2" s="20"/>
       <c r="V2" s="20"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="20">
         <v>2</v>
       </c>
       <c r="D3" s="20"/>
-      <c r="E3" s="20">
-        <v>3</v>
-      </c>
+      <c r="E3" s="20"/>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+      <c r="I3" s="20">
+        <v>3</v>
+      </c>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
@@ -677,86 +742,106 @@
       <c r="T3" s="20"/>
       <c r="U3" s="20"/>
       <c r="V3" s="20"/>
-    </row>
-    <row r="4" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="21">
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+    </row>
+    <row r="4" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="18">
+        <v>24</v>
+      </c>
+      <c r="D4" s="18">
+        <v>25</v>
+      </c>
+      <c r="E4" s="18">
+        <v>26</v>
+      </c>
+      <c r="F4" s="18">
+        <v>27</v>
+      </c>
+      <c r="G4" s="18">
         <v>28</v>
       </c>
-      <c r="D4" s="22">
+      <c r="H4" s="19">
         <v>29</v>
       </c>
-      <c r="E4" s="22">
+      <c r="I4" s="19">
         <v>1</v>
       </c>
-      <c r="F4" s="22">
+      <c r="J4" s="19">
         <v>2</v>
       </c>
-      <c r="G4" s="22">
+      <c r="K4" s="19">
         <v>3</v>
       </c>
-      <c r="H4" s="22">
+      <c r="L4" s="19">
         <v>4</v>
       </c>
-      <c r="I4" s="22">
+      <c r="M4" s="19">
         <v>5</v>
       </c>
-      <c r="J4" s="22">
+      <c r="N4" s="19">
         <v>6</v>
       </c>
-      <c r="K4" s="22">
+      <c r="O4" s="19">
         <v>7</v>
       </c>
-      <c r="L4" s="22">
+      <c r="P4" s="19">
         <v>8</v>
       </c>
-      <c r="M4" s="22">
+      <c r="Q4" s="19">
         <v>9</v>
       </c>
-      <c r="N4" s="22">
+      <c r="R4" s="19">
         <v>10</v>
       </c>
-      <c r="O4" s="22">
+      <c r="S4" s="19">
         <v>11</v>
       </c>
-      <c r="P4" s="22">
+      <c r="T4" s="19">
         <v>12</v>
       </c>
-      <c r="Q4" s="22">
+      <c r="U4" s="19">
         <v>13</v>
       </c>
-      <c r="R4" s="22">
+      <c r="V4" s="19">
         <v>14</v>
       </c>
-      <c r="S4" s="22">
+      <c r="W4" s="19">
         <v>15</v>
       </c>
-      <c r="T4" s="22">
+      <c r="X4" s="19">
         <v>16</v>
       </c>
-      <c r="U4" s="22">
+      <c r="Y4" s="19">
         <v>17</v>
       </c>
-      <c r="V4" s="22">
+      <c r="Z4" s="19">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>0</v>
+      <c r="AA4" s="19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="19">
+        <v>1</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -769,13 +854,18 @@
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>1</v>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>2</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -788,50 +878,60 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>2</v>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
+        <v>3</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>3</v>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="30"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>4</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -840,26 +940,31 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>4</v>
+      <c r="J8" s="2"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
+        <v>5</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -868,82 +973,97 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>5</v>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <v>6</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>6</v>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="19">
+        <v>7</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="24"/>
+      <c r="AA11" s="24"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
+        <v>8</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -951,83 +1071,98 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="10"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="19">
+        <v>9</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>8</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>26</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>10</v>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
+        <v>11</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1038,24 +1173,29 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>11</v>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="23"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="19">
+        <v>12</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1068,22 +1208,27 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>12</v>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
+      <c r="AA16" s="25"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
+        <v>13</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1093,25 +1238,30 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>13</v>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="27"/>
+      <c r="Y17" s="27"/>
+      <c r="Z17" s="27"/>
+      <c r="AA17" s="27"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="19">
+        <v>14</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1120,26 +1270,31 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>14</v>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="17"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
+        <v>15</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1155,19 +1310,24 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>15</v>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
+        <v>16</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1179,25 +1339,393 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="17"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="26"/>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="26"/>
+      <c r="AA20" s="26"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="19">
+        <v>17</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
+      <c r="AA21" s="12"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="19">
+        <v>18</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" s="19">
+        <v>19</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="14"/>
+      <c r="X23" s="14"/>
+      <c r="Y23" s="14"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="14"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" s="19">
+        <v>20</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="19">
+        <v>21</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="16"/>
+      <c r="AA25" s="16"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" s="19">
+        <v>22</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="28"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="19">
+        <v>23</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" s="19">
+        <v>24</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
+      <c r="U28" s="29"/>
+      <c r="V28" s="29"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="29"/>
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29"/>
+      <c r="AA28" s="29"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" s="19">
+        <v>25</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="22"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30" s="19">
+        <v>26</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
+      <c r="Z30" s="13"/>
+      <c r="AA30" s="13"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31" s="19">
+        <v>27</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
+      <c r="AA31" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C1:V1"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="A1:A4"/>
-    <mergeCell ref="E3:V3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C2:V2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:AA3"/>
+    <mergeCell ref="C2:AA2"/>
+    <mergeCell ref="C1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>